<commit_message>
seeding updated, error removed
</commit_message>
<xml_diff>
--- a/db/dummydata/3_PUBLIC_ocean_ptp_rates.xlsx
+++ b/db/dummydata/3_PUBLIC_ocean_ptp_rates.xlsx
@@ -119,7 +119,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="D&quot;. &quot;MMM&quot;. &quot;YYYY"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -144,6 +144,9 @@
       <sz val="10.0"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -159,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -198,6 +201,18 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1213,68 +1228,68 @@
       <c r="AE13" s="10"/>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14">
         <v>43101.0</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="15">
         <v>43465.0</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="12">
         <v>20.0</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="12">
         <v>1.5</v>
       </c>
-      <c r="I14" s="11">
+      <c r="I14" s="12">
         <v>5.0</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="12">
         <v>4.0</v>
       </c>
-      <c r="K14" s="10" t="s">
+      <c r="K14" s="16" t="s">
         <v>24</v>
       </c>
       <c r="L14" s="12">
         <v>650.0</v>
       </c>
-      <c r="M14" s="11">
+      <c r="M14" s="12">
         <v>5.0</v>
       </c>
-      <c r="N14" s="10">
+      <c r="N14" s="12">
         <v>4.0</v>
       </c>
-      <c r="O14" s="10" t="s">
+      <c r="O14" s="16" t="s">
         <v>24</v>
       </c>
       <c r="P14" s="12">
         <v>980.0</v>
       </c>
-      <c r="Q14" s="11">
+      <c r="Q14" s="12">
         <v>5.0</v>
       </c>
-      <c r="R14" s="10">
+      <c r="R14" s="12">
         <v>4.0</v>
       </c>
-      <c r="S14" s="10" t="s">
+      <c r="S14" s="16" t="s">
         <v>24</v>
       </c>
       <c r="T14" s="12">
         <v>1180.0</v>
       </c>
-      <c r="U14" s="11">
+      <c r="U14" s="12">
         <v>5.0</v>
       </c>
-      <c r="V14" s="10">
+      <c r="V14" s="12">
         <v>4.0</v>
       </c>
       <c r="W14" s="10"/>
@@ -1288,68 +1303,68 @@
       <c r="AE14" s="10"/>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8">
+      <c r="A15" s="13"/>
+      <c r="B15" s="14">
         <v>43101.0</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="15">
         <v>43465.0</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="12">
         <v>20.0</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="12">
         <v>1.5</v>
       </c>
-      <c r="I15" s="11">
+      <c r="I15" s="12">
         <v>5.0</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="12">
         <v>4.0</v>
       </c>
-      <c r="K15" s="10" t="s">
+      <c r="K15" s="16" t="s">
         <v>24</v>
       </c>
       <c r="L15" s="12">
         <v>650.0</v>
       </c>
-      <c r="M15" s="11">
+      <c r="M15" s="12">
         <v>5.0</v>
       </c>
-      <c r="N15" s="10">
+      <c r="N15" s="12">
         <v>4.0</v>
       </c>
-      <c r="O15" s="10" t="s">
+      <c r="O15" s="16" t="s">
         <v>24</v>
       </c>
       <c r="P15" s="12">
         <v>980.0</v>
       </c>
-      <c r="Q15" s="11">
+      <c r="Q15" s="12">
         <v>5.0</v>
       </c>
-      <c r="R15" s="10">
+      <c r="R15" s="12">
         <v>4.0</v>
       </c>
-      <c r="S15" s="10" t="s">
+      <c r="S15" s="16" t="s">
         <v>24</v>
       </c>
       <c r="T15" s="12">
         <v>1180.0</v>
       </c>
-      <c r="U15" s="11">
+      <c r="U15" s="12">
         <v>5.0</v>
       </c>
-      <c r="V15" s="10">
+      <c r="V15" s="12">
         <v>4.0</v>
       </c>
       <c r="W15" s="10"/>
@@ -1363,68 +1378,68 @@
       <c r="AE15" s="10"/>
     </row>
     <row r="16" ht="13.5" customHeight="1">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8">
+      <c r="A16" s="13"/>
+      <c r="B16" s="14">
         <v>43101.0</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="15">
         <v>43465.0</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="12">
         <v>20.0</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="12">
         <v>1.5</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="12">
         <v>5.0</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="12">
         <v>4.0</v>
       </c>
-      <c r="K16" s="10" t="s">
+      <c r="K16" s="16" t="s">
         <v>24</v>
       </c>
       <c r="L16" s="12">
         <v>650.0</v>
       </c>
-      <c r="M16" s="11">
+      <c r="M16" s="12">
         <v>5.0</v>
       </c>
-      <c r="N16" s="10">
+      <c r="N16" s="12">
         <v>4.0</v>
       </c>
-      <c r="O16" s="10" t="s">
+      <c r="O16" s="16" t="s">
         <v>24</v>
       </c>
       <c r="P16" s="12">
         <v>980.0</v>
       </c>
-      <c r="Q16" s="11">
+      <c r="Q16" s="12">
         <v>5.0</v>
       </c>
-      <c r="R16" s="10">
+      <c r="R16" s="12">
         <v>4.0</v>
       </c>
-      <c r="S16" s="10" t="s">
+      <c r="S16" s="16" t="s">
         <v>24</v>
       </c>
       <c r="T16" s="12">
         <v>1180.0</v>
       </c>
-      <c r="U16" s="11">
+      <c r="U16" s="12">
         <v>5.0</v>
       </c>
-      <c r="V16" s="10">
+      <c r="V16" s="12">
         <v>4.0</v>
       </c>
       <c r="W16" s="10"/>
@@ -1438,68 +1453,68 @@
       <c r="AE16" s="10"/>
     </row>
     <row r="17" ht="13.5" customHeight="1">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8">
+      <c r="A17" s="13"/>
+      <c r="B17" s="14">
         <v>43101.0</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="15">
         <v>43465.0</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="12">
         <v>20.0</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="12">
         <v>1.5</v>
       </c>
-      <c r="I17" s="11">
+      <c r="I17" s="12">
         <v>5.0</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="12">
         <v>4.0</v>
       </c>
-      <c r="K17" s="10" t="s">
+      <c r="K17" s="16" t="s">
         <v>24</v>
       </c>
       <c r="L17" s="12">
         <v>650.0</v>
       </c>
-      <c r="M17" s="11">
+      <c r="M17" s="12">
         <v>5.0</v>
       </c>
-      <c r="N17" s="10">
+      <c r="N17" s="12">
         <v>4.0</v>
       </c>
-      <c r="O17" s="10" t="s">
+      <c r="O17" s="16" t="s">
         <v>24</v>
       </c>
       <c r="P17" s="12">
         <v>980.0</v>
       </c>
-      <c r="Q17" s="11">
+      <c r="Q17" s="12">
         <v>5.0</v>
       </c>
-      <c r="R17" s="10">
+      <c r="R17" s="12">
         <v>4.0</v>
       </c>
-      <c r="S17" s="10" t="s">
+      <c r="S17" s="16" t="s">
         <v>24</v>
       </c>
       <c r="T17" s="12">
         <v>1180.0</v>
       </c>
-      <c r="U17" s="11">
+      <c r="U17" s="12">
         <v>5.0</v>
       </c>
-      <c r="V17" s="10">
+      <c r="V17" s="12">
         <v>4.0</v>
       </c>
       <c r="W17" s="10"/>

</xml_diff>